<commit_message>
minor fix to project and docs
</commit_message>
<xml_diff>
--- a/ProdutBacklog.xlsx
+++ b/ProdutBacklog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ISS_TemaFinale\iss2019TemaFinale\Analisi Iniziale\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ISS_TemaFinale\iss2019TemaFinale\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C421FD60-23D9-4CD6-9037-0F1E9701A9BE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428B77F7-B7E9-4FDE-AA87-670B4B90FF15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="68">
   <si>
     <t>Tag</t>
   </si>
@@ -63,9 +63,6 @@
     <t>NOTIFY</t>
   </si>
   <si>
-    <t>Tag uguali per requisiti diversi ma simmetrici</t>
-  </si>
-  <si>
     <t>ANSWER</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
     <t>Come RBR devo essere in grado di calcolare le dimensioni della stanza</t>
   </si>
   <si>
-    <t>Come RBR devo conoscere le posizioni degli oggetti nella stanza</t>
-  </si>
-  <si>
     <t>Come RBR devo poter riconoscere ed evitare gli ostacoli</t>
   </si>
   <si>
@@ -205,6 +199,36 @@
   </si>
   <si>
     <t>EXHIBIT</t>
+  </si>
+  <si>
+    <t>Come RBR devo individuare la posizione del tavolo nella stanza</t>
+  </si>
+  <si>
+    <t>Come Pantry devo permettere l'inserimento di piatti</t>
+  </si>
+  <si>
+    <t>Come Pantry devo permettere la rimozione di piatti</t>
+  </si>
+  <si>
+    <t>Come Dishwasher devo permettere l'inserimento di piatti</t>
+  </si>
+  <si>
+    <t>Come Dishwasher devo permettere la rimozione di piatti</t>
+  </si>
+  <si>
+    <t>Come Table devo permettere l'inserimento di piatti/cibo</t>
+  </si>
+  <si>
+    <t>PUT_P</t>
+  </si>
+  <si>
+    <t>TAKE_D</t>
+  </si>
+  <si>
+    <t>Come Table devo permettere la rimozione di piatti/cibo</t>
+  </si>
+  <si>
+    <t>PRODUCT BACKLOG</t>
   </si>
 </sst>
 </file>
@@ -220,7 +244,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -230,18 +254,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -264,13 +276,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -551,20 +564,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:F41"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="91.5703125" customWidth="1"/>
+    <col min="2" max="2" width="81.85546875" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -574,250 +592,422 @@
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>40</v>
       </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>42</v>
-      </c>
       <c r="B6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="C6" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="C7" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="C9" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="C10" s="4">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="C11" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C14" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="C15" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>47</v>
       </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="B19" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="C20" s="4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="4"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="C27" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="4"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>57</v>
-      </c>
-      <c r="B26" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>56</v>
-      </c>
-      <c r="B27" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>58</v>
-      </c>
-      <c r="B28" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B31" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32" t="s">
-        <v>39</v>
+      <c r="C32" s="4">
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="C33" s="4">
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+      <c r="C34" s="4">
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>5</v>
       </c>
+      <c r="C35" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C36" s="4"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C39" s="4"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>65</v>
+      </c>
+      <c r="B41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="4">
+        <v>2</v>
+      </c>
       <c r="D41" s="2"/>
     </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C42" s="4"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" t="s">
+        <v>63</v>
+      </c>
+      <c r="C43" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" t="s">
+        <v>66</v>
+      </c>
+      <c r="C44" s="4">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>